<commit_message>
Update API Status and Collections
Update API Status and Collections
</commit_message>
<xml_diff>
--- a/HealthHub-Api-Details.xlsx
+++ b/HealthHub-Api-Details.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">Eid,VistiDate, Hospital, DoctorName, CaseDetails, ReportName, FileId    </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>S.No</t>
   </si>
@@ -56,25 +53,12 @@
     <t>Get Details From UserId</t>
   </si>
   <si>
-    <t>Get Report Details</t>
-  </si>
-  <si>
     <t>Validate Hospital User</t>
   </si>
   <si>
     <t>Create Hospital Entry</t>
   </si>
   <si>
-    <t>EID Validation, fromDate and Todate  - (Get Details From UserId)</t>
-  </si>
-  <si>
-    <t>New Add/ Modify Add - Done</t>
-  </si>
-  <si>
-    <t>Get Specific Case Report Details 
-(Eid,VistiDate, Hospital, DoctorName)</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -94,13 +78,97 @@
   </si>
   <si>
     <t>Get User Details</t>
+  </si>
+  <si>
+    <t>Create Visit Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Case/Visit Creation </t>
+  </si>
+  <si>
+    <t>Get Visit Details by UserID</t>
+  </si>
+  <si>
+    <t>Get Visit Details By UserId</t>
+  </si>
+  <si>
+    <t>Get Visit Details By Date Range</t>
+  </si>
+  <si>
+    <t>Create Report Details</t>
+  </si>
+  <si>
+    <t>Upload File</t>
+  </si>
+  <si>
+    <t>Download a File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get All Records for the Specigic Visit </t>
+  </si>
+  <si>
+    <t>Create Reports for Specific Visit and File Id</t>
+  </si>
+  <si>
+    <t>Get Report Details By VisitId</t>
+  </si>
+  <si>
+    <t>Get Visit Details by EID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Get Visit Details Eid</t>
+  </si>
+  <si>
+    <t>Get Visit Details Eid and Date Range</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/eid/getByEid/72919812345678</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/user/create</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/user/validateUserId</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/user/getByUserId/therathna</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/visit/create</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/visit/getByUserID/therathna</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/visit/getByEid/7291984123456789</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/file/upload</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/file/download/613fc91155c59b109a806a93</t>
+  </si>
+  <si>
+    <t>Upload a file</t>
+  </si>
+  <si>
+    <t>Download a file by fileUploadId</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/report/create</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/report/getByVisitId/61448d8c44e88c6aafc53b93</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +180,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,19 +249,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -199,8 +273,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,178 +558,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="E6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="C19" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>